<commit_message>
ultimos cambios en el contrato
</commit_message>
<xml_diff>
--- a/Empeño.WindowsForms/Empeños/Comprobantes/ContratoEmpeños.xlsx
+++ b/Empeño.WindowsForms/Empeños/Comprobantes/ContratoEmpeños.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtjarquinm\Documents\GitHub-Donovan\Empe-o\Empeño.WindowsForms\Empeños\Comprobantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC4031D-B369-4511-B878-9E5ADDA7040A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82497EEC-F9C1-4260-A608-2AE37D8F41A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,17 +157,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,11 +175,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,8 +469,8 @@
   </sheetPr>
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,58 +481,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="44.5" x14ac:dyDescent="0.85">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="122.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A8" s="1"/>
@@ -544,483 +544,483 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
     </row>
     <row r="58" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
     </row>
     <row r="59" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
     </row>
     <row r="60" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
     </row>
     <row r="61" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
     </row>
     <row r="63" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
     </row>
     <row r="66" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
+      <c r="A68" s="10"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
     </row>
     <row r="69" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
+      <c r="A69" s="10"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
     </row>
     <row r="70" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
     </row>
     <row r="71" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
     </row>
     <row r="73" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
     </row>
     <row r="75" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
+      <c r="A75" s="10"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
+      <c r="A77" s="10"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
     </row>
     <row r="78" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
+      <c r="A78" s="10"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
     </row>
     <row r="79" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
+      <c r="A79" s="10"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
     </row>
     <row r="80" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
     </row>
     <row r="81" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
+      <c r="A81" s="10"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
     </row>
     <row r="82" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="12"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
+      <c r="A82" s="10"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
     </row>
     <row r="83" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
     </row>
     <row r="84" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
     </row>
     <row r="85" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="12"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
+      <c r="A86" s="10"/>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
     </row>
     <row r="87" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
     </row>
     <row r="88" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A88" s="3"/>
@@ -1038,44 +1038,44 @@
     </row>
     <row r="90" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="91" spans="1:5" ht="60" x14ac:dyDescent="1.1499999999999999">
-      <c r="A91" s="8"/>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
     </row>
     <row r="92" spans="1:5" ht="60" x14ac:dyDescent="0.35">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
     </row>
     <row r="94" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="9"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="9"/>
-      <c r="D94" s="9"/>
+      <c r="A94" s="8"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="9"/>
-      <c r="D95" s="9"/>
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
     </row>
     <row r="96" spans="1:5" ht="60" x14ac:dyDescent="1.1499999999999999">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>